<commit_message>
(dev, Python ipynb)Parte I EDA
</commit_message>
<xml_diff>
--- a/FAII/Talleres/Taller_Practico/data/Diccionario.xlsx
+++ b/FAII/Talleres/Taller_Practico/data/Diccionario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Clases\ICESI\2024_I\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10 Pro\OneDrive - Universidad Icesi\MAESTRIA DATOS )\SEMESTRE II\FUNDAMENTOS DE ANÁLITICA\SEGUNDA PARTE\REPOSITORIO GIT\FAII\Talleres\Taller_Practico\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF96959-91E5-442C-B911-AB8102AF9508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C184F1-43EC-4A9A-88D2-0B7A850A6693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -615,16 +615,16 @@
   <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="59.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
@@ -632,7 +632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -640,7 +640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -648,7 +648,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -656,7 +656,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -664,7 +664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -672,7 +672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -680,7 +680,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -688,7 +688,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -696,7 +696,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -704,7 +704,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -712,7 +712,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -720,7 +720,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -728,7 +728,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -736,7 +736,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -744,7 +744,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -752,7 +752,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -760,7 +760,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -768,7 +768,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -776,7 +776,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -784,7 +784,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -792,7 +792,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -800,7 +800,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -808,7 +808,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -816,7 +816,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -824,7 +824,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -832,7 +832,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -840,7 +840,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>45</v>
       </c>
@@ -848,7 +848,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -856,7 +856,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -864,7 +864,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>51</v>
       </c>
@@ -872,7 +872,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -880,7 +880,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -888,7 +888,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>57</v>
       </c>
@@ -896,7 +896,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -904,7 +904,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -912,7 +912,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -920,7 +920,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -928,7 +928,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>67</v>
       </c>
@@ -936,7 +936,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -944,7 +944,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>71</v>
       </c>
@@ -952,7 +952,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>73</v>
       </c>
@@ -960,7 +960,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -968,7 +968,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>77</v>
       </c>

</xml_diff>

<commit_message>
[Continuación visualización de datos]
</commit_message>
<xml_diff>
--- a/FAII/Talleres/Taller_Practico/data/Diccionario.xlsx
+++ b/FAII/Talleres/Taller_Practico/data/Diccionario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Windows 10 Pro\OneDrive - Universidad Icesi\MAESTRIA DATOS )\SEMESTRE II\FUNDAMENTOS DE ANÁLITICA\SEGUNDA PARTE\REPOSITORIO GIT\FAII\Talleres\Taller_Practico\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8225E867-1CEE-4E4E-A3AE-DBAF36ED20E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357E3943-03AC-46A5-A05A-E88203B008B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16950" yWindow="345" windowWidth="11850" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -385,16 +385,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:B27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,13 +894,13 @@
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="3" t="s">
         <v>99</v>
       </c>
       <c r="D20" t="s">
@@ -914,7 +914,7 @@
       <c r="B21" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="6" t="s">
         <v>92</v>
       </c>
     </row>
@@ -925,7 +925,7 @@
       <c r="B22" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C22" s="3"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -934,7 +934,7 @@
       <c r="B23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="3"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
@@ -943,7 +943,7 @@
       <c r="B24" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="3"/>
+      <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
@@ -952,7 +952,7 @@
       <c r="B25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C25" s="3"/>
+      <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -961,7 +961,7 @@
       <c r="B26" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -970,7 +970,7 @@
       <c r="B27" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="3"/>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -997,33 +997,35 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="5" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>57</v>
       </c>
@@ -1031,7 +1033,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>59</v>
       </c>
@@ -1039,7 +1041,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -1047,7 +1049,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -1055,7 +1057,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -1063,7 +1065,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>67</v>
       </c>
@@ -1071,7 +1073,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -1079,7 +1081,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>71</v>
       </c>
@@ -1087,7 +1089,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>73</v>
       </c>
@@ -1095,7 +1097,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -1103,7 +1105,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>77</v>
       </c>
@@ -1112,10 +1114,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="C10:C13"/>
     <mergeCell ref="C21:C27"/>
+    <mergeCell ref="C31:C33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>